<commit_message>
added imported terms from CL, CLO, UBERON. Changed metadata
</commit_message>
<xml_diff>
--- a/miago/docs/python code/data/transfering_assumption.xlsx
+++ b/miago/docs/python code/data/transfering_assumption.xlsx
@@ -15,7 +15,7 @@
     <sheet name="test" sheetId="1" r:id="rId1"/>
     <sheet name="assay_tissue_organism_mapping" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -10088,8 +10088,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q1042"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L400" workbookViewId="0">
-      <selection activeCell="L404" sqref="A404:XFD404"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
reset the tree of files. Added al the owl files into pre-release miago.owl
</commit_message>
<xml_diff>
--- a/miago/docs/python code/data/transfering_assumption.xlsx
+++ b/miago/docs/python code/data/transfering_assumption.xlsx
@@ -10086,8 +10086,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q1042"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M10" workbookViewId="0">
-      <selection activeCell="O23" sqref="O23"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="M51" sqref="M51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>